<commit_message>
update: added columns back to lassa & rerun to generate results & db
</commit_message>
<xml_diff>
--- a/Pubmed/Lassa/ReferenceSummary_Genbank_Feb19.xlsx
+++ b/Pubmed/Lassa/ReferenceSummary_Genbank_Feb19.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindazhou/Dropbox/___SystematicReviewsAI/LASV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindazhou/Desktop/HIV/GenBankRefs/Pubmed/Lassa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B4CD3D-D87F-2146-BCBD-3DC4EECF054A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF7DA06-18BE-794B-8A2B-F5B42DEA6667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="2160" windowWidth="34560" windowHeight="20080" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
+    <workbookView xWindow="5140" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Authors</t>
   </si>
@@ -163,34 +163,10 @@
     <t>AY216502, AY216503, AY216504, AY216505, AY216506, AY216507, AY216508, AY216509, AY216510, AY216511, AY216513, AY216514, AY216515, AY216516, AY216517, AY216518, AY216519, and AY216520.</t>
   </si>
   <si>
-    <t>LASV</t>
-  </si>
-  <si>
-    <t>X52400</t>
-  </si>
-  <si>
     <t>Sierra Leone</t>
   </si>
   <si>
     <t>L, N, GPC</t>
-  </si>
-  <si>
-    <t>Nucleotide sequence of the S RNA of Lassa virus (Nigerian strain) and comparative analysis of arenavirus gene products</t>
-  </si>
-  <si>
-    <t>Clegg JC, Wilson SM, Oram JD</t>
-  </si>
-  <si>
-    <t>Virus Research</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homo sapiens </t>
-  </si>
-  <si>
-    <t>GPC, N</t>
   </si>
 </sst>
 </file>
@@ -658,11 +634,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4482E4AD-E7FE-EC42-9928-56B66BBA47E4}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomLeft" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -827,7 +803,7 @@
         <v>32</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>39</v>
@@ -839,51 +815,7 @@
         <v>36</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1990</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2042397</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="1">
-        <v>1990</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: rerun lassa after adding back 1 paper
</commit_message>
<xml_diff>
--- a/Pubmed/Lassa/ReferenceSummary_Genbank_Feb19.xlsx
+++ b/Pubmed/Lassa/ReferenceSummary_Genbank_Feb19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindazhou/Desktop/HIV/GenBankRefs/Pubmed/Lassa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF7DA06-18BE-794B-8A2B-F5B42DEA6667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089A9EB8-0285-A044-8928-769CE8C10748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
+    <workbookView xWindow="420" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Authors</t>
   </si>
@@ -167,6 +167,36 @@
   </si>
   <si>
     <t>L, N, GPC</t>
+  </si>
+  <si>
+    <t>Clegg JC.</t>
+  </si>
+  <si>
+    <t>Curr Top Microbiol Immunol. 2002;262:1-24. doi: 10.1007/978-3-642-56029-3_1.</t>
+  </si>
+  <si>
+    <t>11987802</t>
+  </si>
+  <si>
+    <t>LASV</t>
+  </si>
+  <si>
+    <t>Homo Sapiens, rodent</t>
+  </si>
+  <si>
+    <t>Nigeria, Sierra Leone, and Liberia</t>
+  </si>
+  <si>
+    <t>X52400</t>
+  </si>
+  <si>
+    <t>G, N</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>Molecular phylogeny of the arenaviruses</t>
   </si>
 </sst>
 </file>
@@ -634,11 +664,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4482E4AD-E7FE-EC42-9928-56B66BBA47E4}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S8" sqref="S8"/>
+      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -818,6 +848,50 @@
         <v>41</v>
       </c>
     </row>
+    <row r="4" spans="1:23" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>2002</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="1">
+        <v>7</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:W1" xr:uid="{4482E4AD-E7FE-EC42-9928-56B66BBA47E4}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W21">

</xml_diff>

<commit_message>
fix: more cleaning for excels, countries
</commit_message>
<xml_diff>
--- a/Pubmed/Lassa/ReferenceSummary_Genbank_Feb19.xlsx
+++ b/Pubmed/Lassa/ReferenceSummary_Genbank_Feb19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindazhou/Desktop/HIV/GenBankRefs/Pubmed/Lassa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089A9EB8-0285-A044-8928-769CE8C10748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3789B1-D632-F649-B29B-5F7978829406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3031CDAD-EDE9-504F-A9EA-0D1529922A9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -141,9 +141,6 @@
     <t>Rodent</t>
   </si>
   <si>
-    <t>West Africa, Central African Republic, Mozambique/Zimbabwe, South America</t>
-  </si>
-  <si>
     <t>U80003 to U80009</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>Molecular phylogeny of the arenaviruses</t>
+  </si>
+  <si>
+    <t>West Africa, Central African Republic, Mozambique, Zimbabwe, South America</t>
   </si>
 </sst>
 </file>
@@ -666,9 +666,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4482E4AD-E7FE-EC42-9928-56B66BBA47E4}">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -792,19 +792,19 @@
         <v>32</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="288" x14ac:dyDescent="0.2">
@@ -827,69 +827,69 @@
         <v>18</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="Q3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>2002</v>
       </c>
       <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="M4" s="1">
         <v>7</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>